<commit_message>
Base de datos filtrada para celula de Cobertura Vegetal
</commit_message>
<xml_diff>
--- a/BD COBERTURA VEGETAL.xlsx
+++ b/BD COBERTURA VEGETAL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57314\Documents\LEONARDO\CAR\CAR 2022\CONTRATO 2 - 2473\INFORMES VTIC\REDES Cobertura vegetal\Bases de datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57314\Documents\LEONARDO\CAR\CODIGOS\WebScraping MinCiencias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5FD0C6-D2F8-4D66-9664-1DFC403AE1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE988801-4D0F-4EBE-AFB4-26988D1FF81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -622,7 +622,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,7 +659,7 @@
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -667,7 +667,7 @@
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -848,10 +848,14 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{D8593F6C-3312-41D3-8DCE-8E5613B85EED}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{328DEBE0-9E1E-43A7-B67F-208C8118F37C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>